<commit_message>
menambah yang belum ditambah
</commit_message>
<xml_diff>
--- a/app/production/compatibility_model/d/dashboard/result/export/data_hasil/b440_2022-11-18.xlsx
+++ b/app/production/compatibility_model/d/dashboard/result/export/data_hasil/b440_2022-11-18.xlsx
@@ -557,7 +557,7 @@
         <v>7</v>
       </c>
       <c r="G5" s="4">
-        <v>0</v>
+        <v>-2419</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -569,18 +569,18 @@
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1">
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="E6" s="1">
-        <v>0</v>
+        <v>117</v>
       </c>
       <c r="F6" s="1">
         <f>E6-D6</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G6" s="1">
         <f>G5+E6</f>
-        <v>0</v>
+        <v>-2302</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -592,18 +592,18 @@
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1">
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="E7" s="1">
-        <v>0</v>
+        <v>114</v>
       </c>
       <c r="F7" s="1">
         <f>E7-D7</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G7" s="1">
         <f>G6+E7</f>
-        <v>0</v>
+        <v>-2188</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -615,18 +615,18 @@
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1">
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="E8" s="1">
-        <v>0</v>
+        <v>106</v>
       </c>
       <c r="F8" s="1">
         <f>E8-D8</f>
-        <v>0</v>
+        <v>-4</v>
       </c>
       <c r="G8" s="1">
         <f>G7+E8</f>
-        <v>0</v>
+        <v>-2082</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -638,18 +638,18 @@
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1">
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="E9" s="1">
-        <v>0</v>
+        <v>119</v>
       </c>
       <c r="F9" s="1">
         <f>E9-D9</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="G9" s="1">
         <f>G8+E9</f>
-        <v>0</v>
+        <v>-1963</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -672,7 +672,7 @@
       </c>
       <c r="G10" s="2">
         <f>G9+E10</f>
-        <v>0</v>
+        <v>-1963</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -695,7 +695,7 @@
       </c>
       <c r="G11" s="2">
         <f>G10+E11</f>
-        <v>0</v>
+        <v>-1963</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -707,18 +707,18 @@
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1">
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="E12" s="1">
-        <v>0</v>
+        <v>125</v>
       </c>
       <c r="F12" s="1">
         <f>E12-D12</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="G12" s="1">
         <f>G11+E12</f>
-        <v>0</v>
+        <v>-1838</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -730,18 +730,18 @@
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1">
-        <v>0</v>
+        <v>144</v>
       </c>
       <c r="E13" s="1">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F13" s="1">
         <f>E13-D13</f>
-        <v>0</v>
+        <v>-24</v>
       </c>
       <c r="G13" s="1">
         <f>G12+E13</f>
-        <v>0</v>
+        <v>-1718</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -753,10 +753,10 @@
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1">
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="E14" s="1">
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="F14" s="1">
         <f>E14-D14</f>
@@ -764,7 +764,7 @@
       </c>
       <c r="G14" s="1">
         <f>G13+E14</f>
-        <v>0</v>
+        <v>-1608</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -776,18 +776,18 @@
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1">
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="E15" s="1">
-        <v>0</v>
+        <v>104</v>
       </c>
       <c r="F15" s="1">
         <f>E15-D15</f>
-        <v>0</v>
+        <v>-6</v>
       </c>
       <c r="G15" s="1">
         <f>G14+E15</f>
-        <v>0</v>
+        <v>-1504</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -799,18 +799,18 @@
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1">
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="E16" s="1">
-        <v>0</v>
+        <v>114</v>
       </c>
       <c r="F16" s="1">
         <f>E16-D16</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G16" s="1">
         <f>G15+E16</f>
-        <v>0</v>
+        <v>-1390</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -833,7 +833,7 @@
       </c>
       <c r="G17" s="2">
         <f>G16+E17</f>
-        <v>0</v>
+        <v>-1390</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -856,7 +856,7 @@
       </c>
       <c r="G18" s="2">
         <f>G17+E18</f>
-        <v>0</v>
+        <v>-1390</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -868,18 +868,18 @@
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1">
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="E19" s="1">
-        <v>0</v>
+        <v>122</v>
       </c>
       <c r="F19" s="1">
         <f>E19-D19</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="G19" s="1">
         <f>G18+E19</f>
-        <v>0</v>
+        <v>-1268</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -891,18 +891,18 @@
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1">
-        <v>0</v>
+        <v>144</v>
       </c>
       <c r="E20" s="1">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="F20" s="1">
         <f>E20-D20</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G20" s="1">
         <f>G19+E20</f>
-        <v>0</v>
+        <v>-1120</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -914,18 +914,18 @@
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1">
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="E21" s="1">
-        <v>0</v>
+        <v>114</v>
       </c>
       <c r="F21" s="1">
         <f>E21-D21</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G21" s="1">
         <f>G20+E21</f>
-        <v>0</v>
+        <v>-1006</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -937,18 +937,18 @@
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1">
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="E22" s="1">
-        <v>0</v>
+        <v>135</v>
       </c>
       <c r="F22" s="1">
         <f>E22-D22</f>
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="G22" s="1">
         <f>G21+E22</f>
-        <v>0</v>
+        <v>-871</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -960,18 +960,18 @@
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="1">
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="E23" s="1">
-        <v>0</v>
+        <v>87</v>
       </c>
       <c r="F23" s="1">
         <f>E23-D23</f>
-        <v>0</v>
+        <v>-23</v>
       </c>
       <c r="G23" s="1">
         <f>G22+E23</f>
-        <v>0</v>
+        <v>-784</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -994,7 +994,7 @@
       </c>
       <c r="G24" s="2">
         <f>G23+E24</f>
-        <v>0</v>
+        <v>-784</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -1017,7 +1017,7 @@
       </c>
       <c r="G25" s="2">
         <f>G24+E25</f>
-        <v>0</v>
+        <v>-784</v>
       </c>
     </row>
     <row r="26" spans="1:7">
@@ -1029,18 +1029,18 @@
       </c>
       <c r="C26" s="1"/>
       <c r="D26" s="1">
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="E26" s="1">
         <v>0</v>
       </c>
       <c r="F26" s="1">
         <f>E26-D26</f>
-        <v>0</v>
+        <v>-110</v>
       </c>
       <c r="G26" s="1">
         <f>G25+E26</f>
-        <v>0</v>
+        <v>-784</v>
       </c>
     </row>
     <row r="27" spans="1:7">
@@ -1052,18 +1052,18 @@
       </c>
       <c r="C27" s="1"/>
       <c r="D27" s="1">
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="E27" s="1">
         <v>0</v>
       </c>
       <c r="F27" s="1">
         <f>E27-D27</f>
-        <v>0</v>
+        <v>-110</v>
       </c>
       <c r="G27" s="1">
         <f>G26+E27</f>
-        <v>0</v>
+        <v>-784</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -1075,18 +1075,18 @@
       </c>
       <c r="C28" s="1"/>
       <c r="D28" s="1">
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="E28" s="1">
         <v>0</v>
       </c>
       <c r="F28" s="1">
         <f>E28-D28</f>
-        <v>0</v>
+        <v>-110</v>
       </c>
       <c r="G28" s="1">
         <f>G27+E28</f>
-        <v>0</v>
+        <v>-784</v>
       </c>
     </row>
     <row r="29" spans="1:7">
@@ -1098,18 +1098,18 @@
       </c>
       <c r="C29" s="1"/>
       <c r="D29" s="1">
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="E29" s="1">
         <v>0</v>
       </c>
       <c r="F29" s="1">
         <f>E29-D29</f>
-        <v>0</v>
+        <v>-110</v>
       </c>
       <c r="G29" s="1">
         <f>G28+E29</f>
-        <v>0</v>
+        <v>-784</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -1121,18 +1121,18 @@
       </c>
       <c r="C30" s="1"/>
       <c r="D30" s="1">
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="E30" s="1">
         <v>0</v>
       </c>
       <c r="F30" s="1">
         <f>E30-D30</f>
-        <v>0</v>
+        <v>-110</v>
       </c>
       <c r="G30" s="1">
         <f>G29+E30</f>
-        <v>0</v>
+        <v>-784</v>
       </c>
     </row>
     <row r="31" spans="1:7">
@@ -1155,7 +1155,7 @@
       </c>
       <c r="G31" s="2">
         <f>G30+E31</f>
-        <v>0</v>
+        <v>-784</v>
       </c>
     </row>
     <row r="32" spans="1:7">
@@ -1178,7 +1178,7 @@
       </c>
       <c r="G32" s="2">
         <f>G31+E32</f>
-        <v>0</v>
+        <v>-784</v>
       </c>
     </row>
     <row r="33" spans="1:7">
@@ -1190,18 +1190,18 @@
       </c>
       <c r="C33" s="1"/>
       <c r="D33" s="1">
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="E33" s="1">
         <v>0</v>
       </c>
       <c r="F33" s="1">
         <f>E33-D33</f>
-        <v>0</v>
+        <v>-110</v>
       </c>
       <c r="G33" s="1">
         <f>G32+E33</f>
-        <v>0</v>
+        <v>-784</v>
       </c>
     </row>
     <row r="34" spans="1:7">
@@ -1213,18 +1213,18 @@
       </c>
       <c r="C34" s="1"/>
       <c r="D34" s="1">
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="E34" s="1">
         <v>0</v>
       </c>
       <c r="F34" s="1">
         <f>E34-D34</f>
-        <v>0</v>
+        <v>-110</v>
       </c>
       <c r="G34" s="1">
         <f>G33+E34</f>
-        <v>0</v>
+        <v>-784</v>
       </c>
     </row>
     <row r="35" spans="1:7">
@@ -1236,18 +1236,18 @@
       </c>
       <c r="C35" s="1"/>
       <c r="D35" s="1">
-        <v>0</v>
+        <v>41</v>
       </c>
       <c r="E35" s="1">
         <v>0</v>
       </c>
       <c r="F35" s="1">
         <f>E35-D35</f>
-        <v>0</v>
+        <v>-41</v>
       </c>
       <c r="G35" s="1">
         <f>G34+E35</f>
-        <v>0</v>
+        <v>-784</v>
       </c>
     </row>
     <row r="36" spans="1:7">
@@ -1267,19 +1267,19 @@
       <c r="C37" s="4"/>
       <c r="D37" s="4">
         <f>SUM(D6:D36)</f>
-        <v>0</v>
+        <v>2419</v>
       </c>
       <c r="E37" s="4">
         <f>SUM(E6:E36)</f>
-        <v>0</v>
+        <v>1635</v>
       </c>
       <c r="F37" s="4">
         <f>SUM(F6:F36)</f>
-        <v>0</v>
+        <v>-784</v>
       </c>
       <c r="G37" s="4">
         <f>E37-D37</f>
-        <v>0</v>
+        <v>-784</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
menambah yang masih conflict dan mengubah yang konflik
te
</commit_message>
<xml_diff>
--- a/app/production/compatibility_model/d/dashboard/result/export/data_hasil/b440_2022-11-18.xlsx
+++ b/app/production/compatibility_model/d/dashboard/result/export/data_hasil/b440_2022-11-18.xlsx
@@ -557,7 +557,7 @@
         <v>7</v>
       </c>
       <c r="G5" s="4">
-        <v>0</v>
+        <v>-2419</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -569,18 +569,18 @@
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1">
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="E6" s="1">
-        <v>0</v>
+        <v>117</v>
       </c>
       <c r="F6" s="1">
         <f>E6-D6</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G6" s="1">
         <f>G5+E6</f>
-        <v>0</v>
+        <v>-2302</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -592,18 +592,18 @@
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1">
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="E7" s="1">
-        <v>0</v>
+        <v>114</v>
       </c>
       <c r="F7" s="1">
         <f>E7-D7</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G7" s="1">
         <f>G6+E7</f>
-        <v>0</v>
+        <v>-2188</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -615,18 +615,18 @@
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1">
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="E8" s="1">
-        <v>0</v>
+        <v>106</v>
       </c>
       <c r="F8" s="1">
         <f>E8-D8</f>
-        <v>0</v>
+        <v>-4</v>
       </c>
       <c r="G8" s="1">
         <f>G7+E8</f>
-        <v>0</v>
+        <v>-2082</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -638,18 +638,18 @@
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1">
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="E9" s="1">
-        <v>0</v>
+        <v>119</v>
       </c>
       <c r="F9" s="1">
         <f>E9-D9</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="G9" s="1">
         <f>G8+E9</f>
-        <v>0</v>
+        <v>-1963</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -672,7 +672,7 @@
       </c>
       <c r="G10" s="2">
         <f>G9+E10</f>
-        <v>0</v>
+        <v>-1963</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -695,7 +695,7 @@
       </c>
       <c r="G11" s="2">
         <f>G10+E11</f>
-        <v>0</v>
+        <v>-1963</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -707,18 +707,18 @@
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1">
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="E12" s="1">
-        <v>0</v>
+        <v>125</v>
       </c>
       <c r="F12" s="1">
         <f>E12-D12</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="G12" s="1">
         <f>G11+E12</f>
-        <v>0</v>
+        <v>-1838</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -730,18 +730,18 @@
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1">
-        <v>0</v>
+        <v>144</v>
       </c>
       <c r="E13" s="1">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F13" s="1">
         <f>E13-D13</f>
-        <v>0</v>
+        <v>-24</v>
       </c>
       <c r="G13" s="1">
         <f>G12+E13</f>
-        <v>0</v>
+        <v>-1718</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -753,10 +753,10 @@
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1">
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="E14" s="1">
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="F14" s="1">
         <f>E14-D14</f>
@@ -764,7 +764,7 @@
       </c>
       <c r="G14" s="1">
         <f>G13+E14</f>
-        <v>0</v>
+        <v>-1608</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -776,18 +776,18 @@
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1">
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="E15" s="1">
-        <v>0</v>
+        <v>104</v>
       </c>
       <c r="F15" s="1">
         <f>E15-D15</f>
-        <v>0</v>
+        <v>-6</v>
       </c>
       <c r="G15" s="1">
         <f>G14+E15</f>
-        <v>0</v>
+        <v>-1504</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -799,18 +799,18 @@
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1">
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="E16" s="1">
-        <v>0</v>
+        <v>114</v>
       </c>
       <c r="F16" s="1">
         <f>E16-D16</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G16" s="1">
         <f>G15+E16</f>
-        <v>0</v>
+        <v>-1390</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -833,7 +833,7 @@
       </c>
       <c r="G17" s="2">
         <f>G16+E17</f>
-        <v>0</v>
+        <v>-1390</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -856,7 +856,7 @@
       </c>
       <c r="G18" s="2">
         <f>G17+E18</f>
-        <v>0</v>
+        <v>-1390</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -868,18 +868,18 @@
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1">
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="E19" s="1">
-        <v>0</v>
+        <v>122</v>
       </c>
       <c r="F19" s="1">
         <f>E19-D19</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="G19" s="1">
         <f>G18+E19</f>
-        <v>0</v>
+        <v>-1268</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -891,18 +891,18 @@
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1">
-        <v>0</v>
+        <v>144</v>
       </c>
       <c r="E20" s="1">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="F20" s="1">
         <f>E20-D20</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G20" s="1">
         <f>G19+E20</f>
-        <v>0</v>
+        <v>-1120</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -914,18 +914,18 @@
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1">
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="E21" s="1">
-        <v>0</v>
+        <v>114</v>
       </c>
       <c r="F21" s="1">
         <f>E21-D21</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G21" s="1">
         <f>G20+E21</f>
-        <v>0</v>
+        <v>-1006</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -937,18 +937,18 @@
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1">
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="E22" s="1">
-        <v>0</v>
+        <v>135</v>
       </c>
       <c r="F22" s="1">
         <f>E22-D22</f>
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="G22" s="1">
         <f>G21+E22</f>
-        <v>0</v>
+        <v>-871</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -960,18 +960,18 @@
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="1">
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="E23" s="1">
-        <v>0</v>
+        <v>87</v>
       </c>
       <c r="F23" s="1">
         <f>E23-D23</f>
-        <v>0</v>
+        <v>-23</v>
       </c>
       <c r="G23" s="1">
         <f>G22+E23</f>
-        <v>0</v>
+        <v>-784</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -994,7 +994,7 @@
       </c>
       <c r="G24" s="2">
         <f>G23+E24</f>
-        <v>0</v>
+        <v>-784</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -1017,7 +1017,7 @@
       </c>
       <c r="G25" s="2">
         <f>G24+E25</f>
-        <v>0</v>
+        <v>-784</v>
       </c>
     </row>
     <row r="26" spans="1:7">
@@ -1029,18 +1029,18 @@
       </c>
       <c r="C26" s="1"/>
       <c r="D26" s="1">
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="E26" s="1">
         <v>0</v>
       </c>
       <c r="F26" s="1">
         <f>E26-D26</f>
-        <v>0</v>
+        <v>-110</v>
       </c>
       <c r="G26" s="1">
         <f>G25+E26</f>
-        <v>0</v>
+        <v>-784</v>
       </c>
     </row>
     <row r="27" spans="1:7">
@@ -1052,18 +1052,18 @@
       </c>
       <c r="C27" s="1"/>
       <c r="D27" s="1">
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="E27" s="1">
         <v>0</v>
       </c>
       <c r="F27" s="1">
         <f>E27-D27</f>
-        <v>0</v>
+        <v>-110</v>
       </c>
       <c r="G27" s="1">
         <f>G26+E27</f>
-        <v>0</v>
+        <v>-784</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -1075,18 +1075,18 @@
       </c>
       <c r="C28" s="1"/>
       <c r="D28" s="1">
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="E28" s="1">
         <v>0</v>
       </c>
       <c r="F28" s="1">
         <f>E28-D28</f>
-        <v>0</v>
+        <v>-110</v>
       </c>
       <c r="G28" s="1">
         <f>G27+E28</f>
-        <v>0</v>
+        <v>-784</v>
       </c>
     </row>
     <row r="29" spans="1:7">
@@ -1098,18 +1098,18 @@
       </c>
       <c r="C29" s="1"/>
       <c r="D29" s="1">
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="E29" s="1">
         <v>0</v>
       </c>
       <c r="F29" s="1">
         <f>E29-D29</f>
-        <v>0</v>
+        <v>-110</v>
       </c>
       <c r="G29" s="1">
         <f>G28+E29</f>
-        <v>0</v>
+        <v>-784</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -1121,18 +1121,18 @@
       </c>
       <c r="C30" s="1"/>
       <c r="D30" s="1">
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="E30" s="1">
         <v>0</v>
       </c>
       <c r="F30" s="1">
         <f>E30-D30</f>
-        <v>0</v>
+        <v>-110</v>
       </c>
       <c r="G30" s="1">
         <f>G29+E30</f>
-        <v>0</v>
+        <v>-784</v>
       </c>
     </row>
     <row r="31" spans="1:7">
@@ -1155,7 +1155,7 @@
       </c>
       <c r="G31" s="2">
         <f>G30+E31</f>
-        <v>0</v>
+        <v>-784</v>
       </c>
     </row>
     <row r="32" spans="1:7">
@@ -1178,7 +1178,7 @@
       </c>
       <c r="G32" s="2">
         <f>G31+E32</f>
-        <v>0</v>
+        <v>-784</v>
       </c>
     </row>
     <row r="33" spans="1:7">
@@ -1190,18 +1190,18 @@
       </c>
       <c r="C33" s="1"/>
       <c r="D33" s="1">
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="E33" s="1">
         <v>0</v>
       </c>
       <c r="F33" s="1">
         <f>E33-D33</f>
-        <v>0</v>
+        <v>-110</v>
       </c>
       <c r="G33" s="1">
         <f>G32+E33</f>
-        <v>0</v>
+        <v>-784</v>
       </c>
     </row>
     <row r="34" spans="1:7">
@@ -1213,18 +1213,18 @@
       </c>
       <c r="C34" s="1"/>
       <c r="D34" s="1">
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="E34" s="1">
         <v>0</v>
       </c>
       <c r="F34" s="1">
         <f>E34-D34</f>
-        <v>0</v>
+        <v>-110</v>
       </c>
       <c r="G34" s="1">
         <f>G33+E34</f>
-        <v>0</v>
+        <v>-784</v>
       </c>
     </row>
     <row r="35" spans="1:7">
@@ -1236,18 +1236,18 @@
       </c>
       <c r="C35" s="1"/>
       <c r="D35" s="1">
-        <v>0</v>
+        <v>41</v>
       </c>
       <c r="E35" s="1">
         <v>0</v>
       </c>
       <c r="F35" s="1">
         <f>E35-D35</f>
-        <v>0</v>
+        <v>-41</v>
       </c>
       <c r="G35" s="1">
         <f>G34+E35</f>
-        <v>0</v>
+        <v>-784</v>
       </c>
     </row>
     <row r="36" spans="1:7">
@@ -1267,19 +1267,19 @@
       <c r="C37" s="4"/>
       <c r="D37" s="4">
         <f>SUM(D6:D36)</f>
-        <v>0</v>
+        <v>2419</v>
       </c>
       <c r="E37" s="4">
         <f>SUM(E6:E36)</f>
-        <v>0</v>
+        <v>1635</v>
       </c>
       <c r="F37" s="4">
         <f>SUM(F6:F36)</f>
-        <v>0</v>
+        <v>-784</v>
       </c>
       <c r="G37" s="4">
         <f>E37-D37</f>
-        <v>0</v>
+        <v>-784</v>
       </c>
     </row>
   </sheetData>

</xml_diff>